<commit_message>
Added in revised ZABOL
</commit_message>
<xml_diff>
--- a/field_submissions/za_expandabilityfactors.xlsx
+++ b/field_submissions/za_expandabilityfactors.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20740" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="ExpFactors" sheetId="6" r:id="rId1"/>
@@ -74,7 +74,7 @@
     <definedName name="WGI_data">#REF!</definedName>
     <definedName name="WGI_WB">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -934,6 +934,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3398,7 +3403,7 @@
       <c r="G108" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="7">
     <mergeCell ref="C92:F92"/>
     <mergeCell ref="C95:F95"/>

</xml_diff>

<commit_message>
Added in revised ZALOC
</commit_message>
<xml_diff>
--- a/field_submissions/za_expandabilityfactors.xlsx
+++ b/field_submissions/za_expandabilityfactors.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20740" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="ExpFactors" sheetId="6" r:id="rId1"/>
@@ -74,7 +74,7 @@
     <definedName name="WGI_data">#REF!</definedName>
     <definedName name="WGI_WB">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -934,11 +934,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -3403,7 +3398,7 @@
       <c r="G108" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="7">
     <mergeCell ref="C92:F92"/>
     <mergeCell ref="C95:F95"/>

</xml_diff>

<commit_message>
Revised ZALOC, Added in ZAHLM
</commit_message>
<xml_diff>
--- a/field_submissions/za_expandabilityfactors.xlsx
+++ b/field_submissions/za_expandabilityfactors.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="ExpFactors" sheetId="6" r:id="rId1"/>
@@ -74,7 +74,7 @@
     <definedName name="WGI_data">#REF!</definedName>
     <definedName name="WGI_WB">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -934,6 +934,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1296,17 +1301,17 @@
       <selection pane="topRight" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="19" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="19" customWidth="1"/>
-    <col min="3" max="6" width="6.5" style="19" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="19" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="19"/>
+    <col min="1" max="1" width="20.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="19" customWidth="1"/>
+    <col min="3" max="6" width="6.42578125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="19" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="45"/>
       <c r="B1" s="45" t="s">
         <v>96</v>
@@ -1325,7 +1330,7 @@
         <v>4.1867999999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1335,7 +1340,7 @@
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:6" ht="14" thickBot="1">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -1345,7 +1350,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="13">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
@@ -1363,7 +1368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -1373,7 +1378,7 @@
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:6" ht="13">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1383,7 +1388,7 @@
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="7" spans="1:6" ht="13">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
@@ -1393,7 +1398,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="13">
+    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -1411,7 +1416,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
@@ -1421,7 +1426,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
     </row>
-    <row r="10" spans="1:6" ht="13">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>16</v>
       </c>
@@ -1431,7 +1436,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="13">
+    <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -1449,7 +1454,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13">
+    <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1467,7 +1472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
@@ -1477,7 +1482,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="13">
+    <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
@@ -1495,7 +1500,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13">
+    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1513,7 +1518,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>19</v>
       </c>
@@ -1523,7 +1528,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="13">
+    <row r="17" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1541,7 +1546,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13">
+    <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>14</v>
       </c>
@@ -1559,7 +1564,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
@@ -1569,7 +1574,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="1:6" ht="13">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>63</v>
       </c>
@@ -1579,7 +1584,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="13">
+    <row r="21" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>58</v>
       </c>
@@ -1597,7 +1602,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>57</v>
       </c>
@@ -1607,7 +1612,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="13">
+    <row r="23" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>74</v>
       </c>
@@ -1625,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13">
+    <row r="24" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>73</v>
       </c>
@@ -1643,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13">
+    <row r="25" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
@@ -1661,7 +1666,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>20</v>
       </c>
@@ -1671,7 +1676,7 @@
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
     </row>
-    <row r="27" spans="1:6" ht="13">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>21</v>
       </c>
@@ -1681,7 +1686,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="13">
+    <row r="28" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>22</v>
       </c>
@@ -1699,7 +1704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>23</v>
       </c>
@@ -1709,7 +1714,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="13">
+    <row r="30" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
@@ -1727,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>24</v>
       </c>
@@ -1737,7 +1742,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" ht="13">
+    <row r="32" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>22</v>
       </c>
@@ -1755,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="13">
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>25</v>
       </c>
@@ -1765,7 +1770,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:9" ht="13">
+    <row r="34" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>22</v>
       </c>
@@ -1783,7 +1788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="13">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>26</v>
       </c>
@@ -1793,7 +1798,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="13">
+    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>22</v>
       </c>
@@ -1811,7 +1816,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="13">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>27</v>
       </c>
@@ -1821,7 +1826,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:9" ht="13">
+    <row r="38" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>22</v>
       </c>
@@ -1839,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="13">
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>9</v>
       </c>
@@ -1849,7 +1854,7 @@
       <c r="E39" s="26"/>
       <c r="F39" s="26"/>
     </row>
-    <row r="40" spans="1:9" ht="13">
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>61</v>
       </c>
@@ -1859,7 +1864,7 @@
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
     </row>
-    <row r="41" spans="1:9" ht="13">
+    <row r="41" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>62</v>
       </c>
@@ -1871,7 +1876,7 @@
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
     </row>
-    <row r="42" spans="1:9" ht="13">
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>28</v>
       </c>
@@ -1894,7 +1899,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="13">
+    <row r="43" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A43" s="43" t="s">
         <v>75</v>
       </c>
@@ -1917,7 +1922,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="13">
+    <row r="44" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A44" s="43" t="s">
         <v>76</v>
       </c>
@@ -1940,7 +1945,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="13">
+    <row r="45" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="43" t="s">
         <v>85</v>
       </c>
@@ -1963,7 +1968,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="13">
+    <row r="46" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="43" t="s">
         <v>77</v>
       </c>
@@ -1986,7 +1991,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="13">
+    <row r="47" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A47" s="43" t="s">
         <v>104</v>
       </c>
@@ -2009,7 +2014,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="13">
+    <row r="48" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A48" s="43" t="s">
         <v>78</v>
       </c>
@@ -2032,7 +2037,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="13">
+    <row r="49" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="43" t="s">
         <v>79</v>
       </c>
@@ -2055,7 +2060,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13">
+    <row r="50" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="44" t="s">
         <v>80</v>
       </c>
@@ -2078,7 +2083,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="13">
+    <row r="51" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="43" t="s">
         <v>81</v>
       </c>
@@ -2101,7 +2106,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13">
+    <row r="52" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A52" s="43" t="s">
         <v>84</v>
       </c>
@@ -2124,7 +2129,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="13">
+    <row r="53" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="43" t="s">
         <v>29</v>
       </c>
@@ -2147,7 +2152,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="13">
+    <row r="54" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="43" t="s">
         <v>86</v>
       </c>
@@ -2170,7 +2175,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="13">
+    <row r="55" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="43" t="s">
         <v>87</v>
       </c>
@@ -2193,7 +2198,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="13">
+    <row r="56" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="43" t="s">
         <v>88</v>
       </c>
@@ -2216,7 +2221,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="13">
+    <row r="57" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="43" t="s">
         <v>89</v>
       </c>
@@ -2239,7 +2244,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="13">
+    <row r="58" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="43" t="s">
         <v>91</v>
       </c>
@@ -2262,7 +2267,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="13">
+    <row r="59" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="43" t="s">
         <v>92</v>
       </c>
@@ -2285,7 +2290,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="13">
+    <row r="60" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="43" t="s">
         <v>93</v>
       </c>
@@ -2308,7 +2313,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="13">
+    <row r="61" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A61" s="43" t="s">
         <v>82</v>
       </c>
@@ -2331,7 +2336,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="13">
+    <row r="62" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A62" s="43" t="s">
         <v>83</v>
       </c>
@@ -2354,7 +2359,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="13">
+    <row r="63" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="43" t="s">
         <v>94</v>
       </c>
@@ -2377,7 +2382,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="13">
+    <row r="64" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A64" s="43" t="s">
         <v>95</v>
       </c>
@@ -2400,7 +2405,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="13">
+    <row r="65" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>90</v>
       </c>
@@ -2423,7 +2428,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="13">
+    <row r="66" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>66</v>
       </c>
@@ -2446,7 +2451,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="13">
+    <row r="67" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
         <v>67</v>
       </c>
@@ -2469,7 +2474,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="13">
+    <row r="68" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
@@ -2492,7 +2497,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="13">
+    <row r="69" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
         <v>31</v>
       </c>
@@ -2515,7 +2520,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="13">
+    <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="32" t="s">
         <v>32</v>
       </c>
@@ -2535,7 +2540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="13">
+    <row r="71" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A71" s="34" t="s">
         <v>33</v>
       </c>
@@ -2561,7 +2566,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="13">
+    <row r="72" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A72" s="34" t="s">
         <v>34</v>
       </c>
@@ -2587,7 +2592,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="13">
+    <row r="73" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A73" s="34" t="s">
         <v>35</v>
       </c>
@@ -2617,7 +2622,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="13">
+    <row r="74" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A74" s="34" t="s">
         <v>36</v>
       </c>
@@ -2643,7 +2648,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="13">
+    <row r="75" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A75" s="34" t="s">
         <v>37</v>
       </c>
@@ -2669,7 +2674,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="13">
+    <row r="76" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A76" s="34" t="s">
         <v>38</v>
       </c>
@@ -2695,7 +2700,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="13">
+    <row r="77" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A77" s="34" t="s">
         <v>39</v>
       </c>
@@ -2721,7 +2726,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="13">
+    <row r="78" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A78" s="34" t="s">
         <v>2</v>
       </c>
@@ -2748,7 +2753,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="13">
+    <row r="79" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A79" s="34" t="s">
         <v>64</v>
       </c>
@@ -2776,7 +2781,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="13">
+    <row r="80" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A80" s="34" t="s">
         <v>69</v>
       </c>
@@ -2802,7 +2807,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="13">
+    <row r="81" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A81" s="34" t="s">
         <v>1</v>
       </c>
@@ -2828,7 +2833,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="13">
+    <row r="82" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
         <v>65</v>
       </c>
@@ -2848,7 +2853,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="13">
+    <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="32" t="s">
         <v>107</v>
       </c>
@@ -2866,7 +2871,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="13">
+    <row r="84" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A84" s="34" t="s">
         <v>109</v>
       </c>
@@ -2890,7 +2895,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="13">
+    <row r="85" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A85" s="34" t="s">
         <v>110</v>
       </c>
@@ -2914,7 +2919,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="13">
+    <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="32" t="s">
         <v>111</v>
       </c>
@@ -2932,7 +2937,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="13">
+    <row r="87" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
         <v>70</v>
       </c>
@@ -2958,7 +2963,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="13">
+    <row r="88" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
         <v>31</v>
       </c>
@@ -2978,7 +2983,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="13">
+    <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="32" t="s">
         <v>40</v>
       </c>
@@ -2996,7 +3001,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="13">
+    <row r="90" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
         <v>41</v>
       </c>
@@ -3017,7 +3022,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="13">
+    <row r="91" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
         <v>42</v>
       </c>
@@ -3043,7 +3048,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="13">
+    <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="32" t="s">
         <v>43</v>
       </c>
@@ -3061,7 +3066,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="13">
+    <row r="93" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A93" s="34" t="s">
         <v>44</v>
       </c>
@@ -3090,7 +3095,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="13">
+    <row r="94" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A94" s="34" t="s">
         <v>45</v>
       </c>
@@ -3110,7 +3115,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="13">
+    <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="32" t="s">
         <v>46</v>
       </c>
@@ -3128,7 +3133,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="13">
+    <row r="96" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A96" s="34" t="s">
         <v>47</v>
       </c>
@@ -3154,7 +3159,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="13">
+    <row r="97" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
         <v>48</v>
       </c>
@@ -3180,7 +3185,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="13">
+    <row r="98" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A98" s="34" t="s">
         <v>49</v>
       </c>
@@ -3206,7 +3211,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="13">
+    <row r="99" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A99" s="34" t="s">
         <v>50</v>
       </c>
@@ -3232,7 +3237,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="13">
+    <row r="100" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A100" s="34" t="s">
         <v>51</v>
       </c>
@@ -3258,7 +3263,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="13">
+    <row r="101" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A101" s="34" t="s">
         <v>52</v>
       </c>
@@ -3284,7 +3289,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="13">
+    <row r="102" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A102" s="34" t="s">
         <v>53</v>
       </c>
@@ -3310,7 +3315,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="13">
+    <row r="103" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="34" t="s">
         <v>54</v>
       </c>
@@ -3336,7 +3341,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="13">
+    <row r="104" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
         <v>55</v>
       </c>
@@ -3362,7 +3367,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="13">
+    <row r="105" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="s">
         <v>56</v>
       </c>
@@ -3388,13 +3393,13 @@
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G106" s="19"/>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G107" s="19"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G108" s="19"/>
     </row>
   </sheetData>

</xml_diff>